<commit_message>
adding additional descriptions for title and description in template
</commit_message>
<xml_diff>
--- a/dist/DIP_Excel_Template.xlsx
+++ b/dist/DIP_Excel_Template.xlsx
@@ -264,7 +264,7 @@
     <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <t>title:
-The official name (title) given to the resource, limited to 255 characters. Acronyms should be used sparingly and only when explained in the description.
+The official name (title) given to the resource, limited to 255 characters and cannot be an empty string (at least 10 characters). Acronyms should be used sparingly and only when explained in the description.
 Example:
 DHS Data Inventory Introduction
 &lt;dcterms:title&gt;</t>
@@ -273,7 +273,7 @@
     <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <t>description:
-A summary of the resource, limited to 4,000 characters.
+A summary of the resource, limited to 4,000 characters. Cannot be an empty string and must be at least 28 characters.
 Example:
 A mission and overview of the Data Inventory Program (DIP) containing instructions, references, terminology, and explanations designed  for users to understand and be able to use the features it contains.
 &lt;dcterms:description&gt;</t>

</xml_diff>